<commit_message>
Further math tests. Excel file for calculating barycentric coordinates and surface heights is now improved.
</commit_message>
<xml_diff>
--- a/BarycentricCoordinates.xlsx
+++ b/BarycentricCoordinates.xlsx
@@ -448,10 +448,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S25"/>
+  <dimension ref="A1:AD25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="AC22" sqref="AC22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -463,7 +463,7 @@
     <col min="10" max="19" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:30">
       <c r="B1" t="s">
         <v>3</v>
       </c>
@@ -477,7 +477,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:30">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -491,13 +491,13 @@
       </c>
       <c r="D2">
         <f>INDEX(J2:S11,10-H5-1,H4+1)</f>
-        <v>1.4</v>
+        <v>1.9149378500000001</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H2" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="J2" s="1">
         <v>90</v>
@@ -529,14 +529,44 @@
       <c r="S2" s="1">
         <v>99</v>
       </c>
-    </row>
-    <row r="3" spans="1:19">
+      <c r="U2">
+        <v>7.7241400000000002</v>
+      </c>
+      <c r="V2">
+        <v>8.2077899999999993</v>
+      </c>
+      <c r="W2">
+        <v>9.1060199999999991</v>
+      </c>
+      <c r="X2">
+        <v>9.24</v>
+      </c>
+      <c r="Y2">
+        <v>9.7172999999999998</v>
+      </c>
+      <c r="Z2">
+        <v>10.6394</v>
+      </c>
+      <c r="AA2">
+        <v>11</v>
+      </c>
+      <c r="AB2">
+        <v>10.535500000000001</v>
+      </c>
+      <c r="AC2">
+        <v>10.081200000000001</v>
+      </c>
+      <c r="AD2">
+        <v>9.8813600000000008</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3">
         <f>(H4+1)*H2</f>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C3">
         <f>(H5+1)*H3</f>
@@ -544,13 +574,13 @@
       </c>
       <c r="D3">
         <f>INDEX(J2:S11,10-H5-1,H4+2)</f>
-        <v>3</v>
+        <v>2.1694214299999999</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>10</v>
       </c>
       <c r="H3" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="J3" s="1">
         <v>80</v>
@@ -582,22 +612,52 @@
       <c r="S3" s="1">
         <v>89</v>
       </c>
-    </row>
-    <row r="4" spans="1:19">
+      <c r="U3">
+        <v>7.1181799999999997</v>
+      </c>
+      <c r="V3">
+        <v>8.3627500000000001</v>
+      </c>
+      <c r="W3">
+        <v>8.8815799999999996</v>
+      </c>
+      <c r="X3">
+        <v>9.0268300000000004</v>
+      </c>
+      <c r="Y3">
+        <v>9.2234300000000005</v>
+      </c>
+      <c r="Z3">
+        <v>10.033099999999999</v>
+      </c>
+      <c r="AA3">
+        <v>10.4359</v>
+      </c>
+      <c r="AB3">
+        <v>10.0405</v>
+      </c>
+      <c r="AC3">
+        <v>9.9442500000000003</v>
+      </c>
+      <c r="AD3">
+        <v>9.7623899999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:30">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4">
         <f>(H4+1)*H2</f>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C4">
         <f>H5*H3</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D4">
         <f>INDEX(J2:S11,10-H5,H4+2)</f>
-        <v>1</v>
+        <v>1.6814620499999999</v>
       </c>
       <c r="G4" t="s">
         <v>11</v>
@@ -636,8 +696,38 @@
       <c r="S4" s="1">
         <v>79</v>
       </c>
-    </row>
-    <row r="5" spans="1:19">
+      <c r="U4">
+        <v>6.4328900000000004</v>
+      </c>
+      <c r="V4">
+        <v>7.6282100000000002</v>
+      </c>
+      <c r="W4">
+        <v>8.8015899999999991</v>
+      </c>
+      <c r="X4">
+        <v>8.4420300000000008</v>
+      </c>
+      <c r="Y4">
+        <v>7.9097400000000002</v>
+      </c>
+      <c r="Z4">
+        <v>8.3754399999999993</v>
+      </c>
+      <c r="AA4">
+        <v>8.5328999999999997</v>
+      </c>
+      <c r="AB4">
+        <v>9.6984100000000009</v>
+      </c>
+      <c r="AC4">
+        <v>9.4666700000000006</v>
+      </c>
+      <c r="AD4">
+        <v>8.6892700000000005</v>
+      </c>
+    </row>
+    <row r="5" spans="1:30">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -647,18 +737,18 @@
       </c>
       <c r="C5">
         <f>H5*H3</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D5">
         <f>INDEX(J2:S11,10-H5,H4+1)</f>
-        <v>0</v>
+        <v>1.1240209299999999</v>
       </c>
       <c r="G5" t="s">
         <v>12</v>
       </c>
       <c r="H5">
         <f>FLOOR(C6/H3,1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J5" s="1">
         <v>60</v>
@@ -690,8 +780,38 @@
       <c r="S5" s="1">
         <v>69</v>
       </c>
-    </row>
-    <row r="6" spans="1:19">
+      <c r="U5">
+        <v>5.15306</v>
+      </c>
+      <c r="V5">
+        <v>6.0157499999999997</v>
+      </c>
+      <c r="W5">
+        <v>7.4549200000000004</v>
+      </c>
+      <c r="X5">
+        <v>7.2142900000000001</v>
+      </c>
+      <c r="Y5">
+        <v>7.8365499999999999</v>
+      </c>
+      <c r="Z5">
+        <v>7.8296000000000001</v>
+      </c>
+      <c r="AA5">
+        <v>7.1428599999999998</v>
+      </c>
+      <c r="AB5">
+        <v>7.3333300000000001</v>
+      </c>
+      <c r="AC5">
+        <v>7.6296299999999997</v>
+      </c>
+      <c r="AD5">
+        <v>7.7142900000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:30">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -731,8 +851,38 @@
       <c r="S6" s="1">
         <v>59</v>
       </c>
-    </row>
-    <row r="7" spans="1:19">
+      <c r="U6">
+        <v>4.1310799999999999</v>
+      </c>
+      <c r="V6">
+        <v>4.7524300000000004</v>
+      </c>
+      <c r="W6">
+        <v>5.3337199999999996</v>
+      </c>
+      <c r="X6">
+        <v>5.3390399999999998</v>
+      </c>
+      <c r="Y6">
+        <v>6.5378800000000004</v>
+      </c>
+      <c r="Z6">
+        <v>7.2430599999999998</v>
+      </c>
+      <c r="AA6">
+        <v>6.96</v>
+      </c>
+      <c r="AB6">
+        <v>6.7254899999999997</v>
+      </c>
+      <c r="AC6">
+        <v>6.4444499999999998</v>
+      </c>
+      <c r="AD6">
+        <v>6.93398</v>
+      </c>
+    </row>
+    <row r="7" spans="1:30">
       <c r="J7" s="1">
         <v>40</v>
       </c>
@@ -763,14 +913,44 @@
       <c r="S7" s="1">
         <v>49</v>
       </c>
-    </row>
-    <row r="8" spans="1:19">
+      <c r="U7">
+        <v>3.9420600000000001</v>
+      </c>
+      <c r="V7">
+        <v>3.8097400000000001</v>
+      </c>
+      <c r="W7">
+        <v>4.2846299999999999</v>
+      </c>
+      <c r="X7">
+        <v>5.0022000000000002</v>
+      </c>
+      <c r="Y7">
+        <v>5.2476200000000004</v>
+      </c>
+      <c r="Z7">
+        <v>4.6969700000000003</v>
+      </c>
+      <c r="AA7">
+        <v>4.6478000000000002</v>
+      </c>
+      <c r="AB7">
+        <v>5.7160500000000001</v>
+      </c>
+      <c r="AC7">
+        <v>5.88889</v>
+      </c>
+      <c r="AD7">
+        <v>5.3121</v>
+      </c>
+    </row>
+    <row r="8" spans="1:30">
       <c r="A8" t="s">
         <v>5</v>
       </c>
       <c r="B8">
         <f>(((C2-C4)*(B3-B4))+((C3-C4)*(B4-B2)))/2</f>
-        <v>50</v>
+        <v>12.5</v>
       </c>
       <c r="J8" s="1">
         <v>30</v>
@@ -802,23 +982,53 @@
       <c r="S8" s="1">
         <v>39</v>
       </c>
-    </row>
-    <row r="9" spans="1:19">
+      <c r="U8">
+        <v>3.23529</v>
+      </c>
+      <c r="V8">
+        <v>2.8014199999999998</v>
+      </c>
+      <c r="W8">
+        <v>2.9716300000000002</v>
+      </c>
+      <c r="X8">
+        <v>3.5714299999999999</v>
+      </c>
+      <c r="Y8">
+        <v>3.5628099999999998</v>
+      </c>
+      <c r="Z8">
+        <v>3.6330900000000002</v>
+      </c>
+      <c r="AA8">
+        <v>3</v>
+      </c>
+      <c r="AB8">
+        <v>4.2415900000000004</v>
+      </c>
+      <c r="AC8">
+        <v>3.9317299999999999</v>
+      </c>
+      <c r="AD8">
+        <v>3.2857099999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:30">
       <c r="A9" t="s">
         <v>6</v>
       </c>
       <c r="B9">
         <f>(((C2-C5)*(B4-B5))+((C4-C5)*(B5-B2)))/2</f>
-        <v>50</v>
+        <v>12.5</v>
       </c>
       <c r="J9" s="1">
-        <v>20</v>
+        <v>1.9149378500000001</v>
       </c>
       <c r="K9" s="1">
-        <v>21</v>
+        <v>2.1694214299999999</v>
       </c>
       <c r="L9" s="1">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="M9" s="1">
         <v>23</v>
@@ -841,23 +1051,53 @@
       <c r="S9" s="1">
         <v>29</v>
       </c>
-    </row>
-    <row r="10" spans="1:19">
+      <c r="U9">
+        <v>2.1865800000000002</v>
+      </c>
+      <c r="V9">
+        <v>1.3596699999999999</v>
+      </c>
+      <c r="W9">
+        <v>1.3777299999999999</v>
+      </c>
+      <c r="X9">
+        <v>1.6666700000000001</v>
+      </c>
+      <c r="Y9">
+        <v>1.2795700000000001</v>
+      </c>
+      <c r="Z9">
+        <v>2.3867400000000001</v>
+      </c>
+      <c r="AA9">
+        <v>2.90055</v>
+      </c>
+      <c r="AB9">
+        <v>3.2544499999999998</v>
+      </c>
+      <c r="AC9">
+        <v>2.7066699999999999</v>
+      </c>
+      <c r="AD9">
+        <v>2.1352899999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:30">
       <c r="A10" t="s">
         <v>16</v>
       </c>
       <c r="B10">
         <f>IF(G12="Top-right triangle",B8,B9)</f>
-        <v>50</v>
+        <v>12.5</v>
       </c>
       <c r="J10" s="1">
-        <v>1.4</v>
+        <v>1.1240209299999999</v>
       </c>
       <c r="K10" s="1">
-        <v>3</v>
+        <v>1.6814620499999999</v>
       </c>
       <c r="L10" s="1">
-        <v>12</v>
+        <v>1.70000017</v>
       </c>
       <c r="M10" s="1">
         <v>13</v>
@@ -880,23 +1120,53 @@
       <c r="S10" s="1">
         <v>19</v>
       </c>
-    </row>
-    <row r="11" spans="1:19">
+      <c r="U10">
+        <v>1.8192600000000001</v>
+      </c>
+      <c r="V10">
+        <v>1.0701799999999999</v>
+      </c>
+      <c r="W10">
+        <v>1.0740700000000001</v>
+      </c>
+      <c r="X10">
+        <v>1.0238700000000001</v>
+      </c>
+      <c r="Y10">
+        <v>0.49019000000000001</v>
+      </c>
+      <c r="Z10">
+        <v>0.62963000000000002</v>
+      </c>
+      <c r="AA10">
+        <v>1.4512100000000001</v>
+      </c>
+      <c r="AB10">
+        <v>1.8676600000000001</v>
+      </c>
+      <c r="AC10">
+        <v>2.44279</v>
+      </c>
+      <c r="AD10">
+        <v>2.0850900000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:30">
       <c r="A11" t="s">
         <v>17</v>
       </c>
       <c r="B11">
         <f>(((C5-C4)*(B6-B4))+((C6-C4)*(B4-B5)))/2</f>
-        <v>31.45</v>
+        <v>3.2250000000000001</v>
       </c>
       <c r="J11" s="1">
         <v>0</v>
       </c>
       <c r="K11" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="L11" s="1">
         <v>1</v>
-      </c>
-      <c r="L11" s="1">
-        <v>2</v>
       </c>
       <c r="M11" s="1">
         <v>3</v>
@@ -919,54 +1189,84 @@
       <c r="S11" s="1">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:19">
+      <c r="U11">
+        <v>1.30769</v>
+      </c>
+      <c r="V11">
+        <v>1.1126199999999999</v>
+      </c>
+      <c r="W11">
+        <v>1.0465100000000001</v>
+      </c>
+      <c r="X11">
+        <v>0.53846000000000005</v>
+      </c>
+      <c r="Y11">
+        <v>8.3059999999999995E-2</v>
+      </c>
+      <c r="Z11">
+        <v>8.8499999999999995E-2</v>
+      </c>
+      <c r="AA11">
+        <v>0.79310000000000003</v>
+      </c>
+      <c r="AB11">
+        <v>1.4761899999999999</v>
+      </c>
+      <c r="AC11">
+        <v>1.81481</v>
+      </c>
+      <c r="AD11">
+        <v>1.9213499999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:30">
       <c r="A12" t="s">
         <v>18</v>
       </c>
       <c r="B12">
         <f>(((C4-C3)*(B6-B3))+((C6-C3)*(B3-B4)))/2</f>
-        <v>32.5</v>
+        <v>3.75</v>
       </c>
       <c r="G12" t="str">
         <f>IF(MOD(B6,H2)/H2&lt;=1-(MOD(C6,H3)/H3),"Bottom-left triangle","Top-right triangle")</f>
         <v>Bottom-left triangle</v>
       </c>
     </row>
-    <row r="13" spans="1:19">
+    <row r="13" spans="1:30">
       <c r="A13" t="s">
         <v>23</v>
       </c>
       <c r="B13">
         <f>IF(G12="Top-right triangle",B12,B11)</f>
-        <v>31.45</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19">
+        <v>3.2250000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:30">
       <c r="A14" t="s">
         <v>21</v>
       </c>
       <c r="B14">
         <f>(((C2-C4)*(B6-B4))+((C6-C4)*(B4-B2)))/2</f>
-        <v>-1.0500000000000007</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19">
+        <v>-0.52499999999999991</v>
+      </c>
+    </row>
+    <row r="15" spans="1:30">
       <c r="A15" t="s">
         <v>19</v>
       </c>
       <c r="B15">
         <f>(((C2-C6)*(B3-B6))+((C3-C6)*(B6-B2)))/2</f>
-        <v>18.549999999999997</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19">
+        <v>9.2749999999999986</v>
+      </c>
+    </row>
+    <row r="16" spans="1:30">
       <c r="A16" t="s">
         <v>20</v>
       </c>
       <c r="B16">
         <f>(((C2-C5)*(B6-B5))+((C6-C5)*(B5-B2)))/2</f>
-        <v>17.5</v>
+        <v>8.75</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -975,7 +1275,7 @@
       </c>
       <c r="B17">
         <f>IF(G12="Top-right triangle",B15,B16)</f>
-        <v>17.5</v>
+        <v>8.75</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -984,7 +1284,7 @@
       </c>
       <c r="B18">
         <f>(((C2-C6)*(B4-B6))+((C4-C6)*(B6-B2)))/2</f>
-        <v>1.0499999999999989</v>
+        <v>0.52499999999999947</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -993,7 +1293,7 @@
       </c>
       <c r="B21">
         <f>B13/B10</f>
-        <v>0.629</v>
+        <v>0.25800000000000001</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -1002,7 +1302,7 @@
       </c>
       <c r="B22">
         <f>IF(G12="Top-right triangle",B14,B18)/B10</f>
-        <v>2.0999999999999977E-2</v>
+        <v>4.1999999999999954E-2</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -1011,7 +1311,7 @@
       </c>
       <c r="B23">
         <f>B17/B10</f>
-        <v>0.35</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -1020,7 +1320,7 @@
       </c>
       <c r="B25">
         <f>D2*B21+IF(G12="Top-right triangle",D3,D5)*B22+D4*B23</f>
-        <v>1.2305999999999999</v>
+        <v>1.71828627936</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improved the excel for barycentric and surface heights calculation.
</commit_message>
<xml_diff>
--- a/BarycentricCoordinates.xlsx
+++ b/BarycentricCoordinates.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="128">
   <si>
     <t>A</t>
   </si>
@@ -100,6 +100,306 @@
   </si>
   <si>
     <t>Barycentric coordinate B2 (opposite B or D)</t>
+  </si>
+  <si>
+    <t>1.30769229</t>
+  </si>
+  <si>
+    <t>1.11262488</t>
+  </si>
+  <si>
+    <t>1.04651153</t>
+  </si>
+  <si>
+    <t>0.538461566</t>
+  </si>
+  <si>
+    <t>0.0830636173</t>
+  </si>
+  <si>
+    <t>0.0885029733</t>
+  </si>
+  <si>
+    <t>0.793103397</t>
+  </si>
+  <si>
+    <t>1.47619081</t>
+  </si>
+  <si>
+    <t>1.81481481</t>
+  </si>
+  <si>
+    <t>1.92134821</t>
+  </si>
+  <si>
+    <t>1.81925511</t>
+  </si>
+  <si>
+    <t>1.07017553</t>
+  </si>
+  <si>
+    <t>1.07407415</t>
+  </si>
+  <si>
+    <t>1.02386630</t>
+  </si>
+  <si>
+    <t>0.490196109</t>
+  </si>
+  <si>
+    <t>0.629629850</t>
+  </si>
+  <si>
+    <t>1.45121014</t>
+  </si>
+  <si>
+    <t>1.86765754</t>
+  </si>
+  <si>
+    <t>2.44278574</t>
+  </si>
+  <si>
+    <t>2.08509278</t>
+  </si>
+  <si>
+    <t>2.18658280</t>
+  </si>
+  <si>
+    <t>1.35966897</t>
+  </si>
+  <si>
+    <t>1.37772787</t>
+  </si>
+  <si>
+    <t>1.66666675</t>
+  </si>
+  <si>
+    <t>1.27957010</t>
+  </si>
+  <si>
+    <t>2.38673568</t>
+  </si>
+  <si>
+    <t>2.90055251</t>
+  </si>
+  <si>
+    <t>3.25445271</t>
+  </si>
+  <si>
+    <t>2.70666671</t>
+  </si>
+  <si>
+    <t>2.13528585</t>
+  </si>
+  <si>
+    <t>3.23529410</t>
+  </si>
+  <si>
+    <t>2.80141854</t>
+  </si>
+  <si>
+    <t>2.97163129</t>
+  </si>
+  <si>
+    <t>3.57142854</t>
+  </si>
+  <si>
+    <t>3.56281376</t>
+  </si>
+  <si>
+    <t>3.63309336</t>
+  </si>
+  <si>
+    <t>3.00000000</t>
+  </si>
+  <si>
+    <t>4.24159098</t>
+  </si>
+  <si>
+    <t>3.93172717</t>
+  </si>
+  <si>
+    <t>3.28571439</t>
+  </si>
+  <si>
+    <t>3.94206190</t>
+  </si>
+  <si>
+    <t>3.80974150</t>
+  </si>
+  <si>
+    <t>4.28462791</t>
+  </si>
+  <si>
+    <t>5.00220060</t>
+  </si>
+  <si>
+    <t>5.24761915</t>
+  </si>
+  <si>
+    <t>4.69696951</t>
+  </si>
+  <si>
+    <t>4.64779902</t>
+  </si>
+  <si>
+    <t>5.71605015</t>
+  </si>
+  <si>
+    <t>5.88888884</t>
+  </si>
+  <si>
+    <t>5.31210136</t>
+  </si>
+  <si>
+    <t>4.13108444</t>
+  </si>
+  <si>
+    <t>4.75242758</t>
+  </si>
+  <si>
+    <t>5.33372402</t>
+  </si>
+  <si>
+    <t>5.33903742</t>
+  </si>
+  <si>
+    <t>6.53787947</t>
+  </si>
+  <si>
+    <t>7.24305582</t>
+  </si>
+  <si>
+    <t>6.96000004</t>
+  </si>
+  <si>
+    <t>6.72549009</t>
+  </si>
+  <si>
+    <t>6.44444513</t>
+  </si>
+  <si>
+    <t>6.93397713</t>
+  </si>
+  <si>
+    <t>5.15306139</t>
+  </si>
+  <si>
+    <t>6.01575422</t>
+  </si>
+  <si>
+    <t>7.45491505</t>
+  </si>
+  <si>
+    <t>7.21428633</t>
+  </si>
+  <si>
+    <t>7.83655453</t>
+  </si>
+  <si>
+    <t>7.82960224</t>
+  </si>
+  <si>
+    <t>7.14285707</t>
+  </si>
+  <si>
+    <t>7.33333349</t>
+  </si>
+  <si>
+    <t>7.62962914</t>
+  </si>
+  <si>
+    <t>7.71428585</t>
+  </si>
+  <si>
+    <t>6.43288612</t>
+  </si>
+  <si>
+    <t>7.62820625</t>
+  </si>
+  <si>
+    <t>8.80158806</t>
+  </si>
+  <si>
+    <t>8.44202900</t>
+  </si>
+  <si>
+    <t>7.90974045</t>
+  </si>
+  <si>
+    <t>8.37543964</t>
+  </si>
+  <si>
+    <t>8.53290272</t>
+  </si>
+  <si>
+    <t>9.69841385</t>
+  </si>
+  <si>
+    <t>9.46666718</t>
+  </si>
+  <si>
+    <t>8.68926620</t>
+  </si>
+  <si>
+    <t>7.11818123</t>
+  </si>
+  <si>
+    <t>8.36275005</t>
+  </si>
+  <si>
+    <t>8.88157654</t>
+  </si>
+  <si>
+    <t>9.02683258</t>
+  </si>
+  <si>
+    <t>9.22342682</t>
+  </si>
+  <si>
+    <t>10.0330791</t>
+  </si>
+  <si>
+    <t>10.4358978</t>
+  </si>
+  <si>
+    <t>10.0404978</t>
+  </si>
+  <si>
+    <t>9.94424725</t>
+  </si>
+  <si>
+    <t>9.76239395</t>
+  </si>
+  <si>
+    <t>7.72413778</t>
+  </si>
+  <si>
+    <t>8.20779228</t>
+  </si>
+  <si>
+    <t>9.10602283</t>
+  </si>
+  <si>
+    <t>9.23999977</t>
+  </si>
+  <si>
+    <t>9.71729946</t>
+  </si>
+  <si>
+    <t>10.6394300</t>
+  </si>
+  <si>
+    <t>11.0000000</t>
+  </si>
+  <si>
+    <t>10.5354986</t>
+  </si>
+  <si>
+    <t>10.0812311</t>
+  </si>
+  <si>
+    <t>9.88135624</t>
   </si>
 </sst>
 </file>
@@ -450,8 +750,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AD25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AC22" sqref="AC22"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="V10" sqref="V10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -461,6 +761,7 @@
     <col min="4" max="4" width="15.5703125" customWidth="1"/>
     <col min="7" max="7" width="21.7109375" customWidth="1"/>
     <col min="10" max="19" width="6.7109375" customWidth="1"/>
+    <col min="21" max="30" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:30">
@@ -491,7 +792,7 @@
       </c>
       <c r="D2">
         <f>INDEX(J2:S11,10-H5-1,H4+1)</f>
-        <v>1.9149378500000001</v>
+        <v>2.1865800000000002</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>9</v>
@@ -500,64 +801,64 @@
         <v>5</v>
       </c>
       <c r="J2" s="1">
-        <v>90</v>
+        <v>7.7241400000000002</v>
       </c>
       <c r="K2" s="1">
-        <v>91</v>
+        <v>8.2077899999999993</v>
       </c>
       <c r="L2" s="1">
-        <v>92</v>
+        <v>9.1060199999999991</v>
       </c>
       <c r="M2" s="1">
-        <v>93</v>
+        <v>9.24</v>
       </c>
       <c r="N2" s="1">
-        <v>94</v>
+        <v>9.7172999999999998</v>
       </c>
       <c r="O2" s="1">
-        <v>95</v>
+        <v>10.6394</v>
       </c>
       <c r="P2" s="1">
-        <v>96</v>
+        <v>11</v>
       </c>
       <c r="Q2" s="1">
-        <v>97</v>
+        <v>10.535500000000001</v>
       </c>
       <c r="R2" s="1">
-        <v>98</v>
+        <v>10.081200000000001</v>
       </c>
       <c r="S2" s="1">
-        <v>99</v>
-      </c>
-      <c r="U2">
-        <v>7.7241400000000002</v>
-      </c>
-      <c r="V2">
-        <v>8.2077899999999993</v>
-      </c>
-      <c r="W2">
-        <v>9.1060199999999991</v>
-      </c>
-      <c r="X2">
-        <v>9.24</v>
-      </c>
-      <c r="Y2">
-        <v>9.7172999999999998</v>
-      </c>
-      <c r="Z2">
-        <v>10.6394</v>
-      </c>
-      <c r="AA2">
-        <v>11</v>
-      </c>
-      <c r="AB2">
-        <v>10.535500000000001</v>
-      </c>
-      <c r="AC2">
-        <v>10.081200000000001</v>
-      </c>
-      <c r="AD2">
         <v>9.8813600000000008</v>
+      </c>
+      <c r="U2" t="s">
+        <v>118</v>
+      </c>
+      <c r="V2" t="s">
+        <v>119</v>
+      </c>
+      <c r="W2" t="s">
+        <v>120</v>
+      </c>
+      <c r="X2" t="s">
+        <v>121</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>122</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>123</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>124</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>125</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>126</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="3" spans="1:30">
@@ -574,7 +875,7 @@
       </c>
       <c r="D3">
         <f>INDEX(J2:S11,10-H5-1,H4+2)</f>
-        <v>2.1694214299999999</v>
+        <v>1.3596699999999999</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>10</v>
@@ -583,64 +884,64 @@
         <v>5</v>
       </c>
       <c r="J3" s="1">
-        <v>80</v>
+        <v>7.1181799999999997</v>
       </c>
       <c r="K3" s="1">
-        <v>81</v>
+        <v>8.3627500000000001</v>
       </c>
       <c r="L3" s="1">
-        <v>82</v>
+        <v>8.8815799999999996</v>
       </c>
       <c r="M3" s="1">
-        <v>83</v>
+        <v>9.0268300000000004</v>
       </c>
       <c r="N3" s="1">
-        <v>84</v>
+        <v>9.2234300000000005</v>
       </c>
       <c r="O3" s="1">
-        <v>85</v>
+        <v>10.033099999999999</v>
       </c>
       <c r="P3" s="1">
-        <v>86</v>
+        <v>10.4359</v>
       </c>
       <c r="Q3" s="1">
-        <v>87</v>
+        <v>10.0405</v>
       </c>
       <c r="R3" s="1">
-        <v>88</v>
+        <v>9.9442500000000003</v>
       </c>
       <c r="S3" s="1">
-        <v>89</v>
-      </c>
-      <c r="U3">
-        <v>7.1181799999999997</v>
-      </c>
-      <c r="V3">
-        <v>8.3627500000000001</v>
-      </c>
-      <c r="W3">
-        <v>8.8815799999999996</v>
-      </c>
-      <c r="X3">
-        <v>9.0268300000000004</v>
-      </c>
-      <c r="Y3">
-        <v>9.2234300000000005</v>
-      </c>
-      <c r="Z3">
-        <v>10.033099999999999</v>
-      </c>
-      <c r="AA3">
-        <v>10.4359</v>
-      </c>
-      <c r="AB3">
-        <v>10.0405</v>
-      </c>
-      <c r="AC3">
-        <v>9.9442500000000003</v>
-      </c>
-      <c r="AD3">
         <v>9.7623899999999999</v>
+      </c>
+      <c r="U3" t="s">
+        <v>108</v>
+      </c>
+      <c r="V3" t="s">
+        <v>109</v>
+      </c>
+      <c r="W3" t="s">
+        <v>110</v>
+      </c>
+      <c r="X3" t="s">
+        <v>111</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>112</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>113</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>114</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>115</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>116</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:30">
@@ -657,7 +958,7 @@
       </c>
       <c r="D4">
         <f>INDEX(J2:S11,10-H5,H4+2)</f>
-        <v>1.6814620499999999</v>
+        <v>1.0701799999999999</v>
       </c>
       <c r="G4" t="s">
         <v>11</v>
@@ -667,64 +968,64 @@
         <v>0</v>
       </c>
       <c r="J4" s="1">
-        <v>70</v>
+        <v>6.4328900000000004</v>
       </c>
       <c r="K4" s="1">
-        <v>71</v>
+        <v>7.6282100000000002</v>
       </c>
       <c r="L4" s="1">
-        <v>72</v>
+        <v>8.8015899999999991</v>
       </c>
       <c r="M4" s="1">
-        <v>73</v>
+        <v>8.4420300000000008</v>
       </c>
       <c r="N4" s="1">
-        <v>74</v>
+        <v>7.9097400000000002</v>
       </c>
       <c r="O4" s="1">
-        <v>75</v>
+        <v>8.3754399999999993</v>
       </c>
       <c r="P4" s="1">
-        <v>76</v>
+        <v>8.5328999999999997</v>
       </c>
       <c r="Q4" s="1">
-        <v>77</v>
+        <v>9.6984100000000009</v>
       </c>
       <c r="R4" s="1">
-        <v>78</v>
+        <v>9.4666700000000006</v>
       </c>
       <c r="S4" s="1">
-        <v>79</v>
-      </c>
-      <c r="U4">
-        <v>6.4328900000000004</v>
-      </c>
-      <c r="V4">
-        <v>7.6282100000000002</v>
-      </c>
-      <c r="W4">
-        <v>8.8015899999999991</v>
-      </c>
-      <c r="X4">
-        <v>8.4420300000000008</v>
-      </c>
-      <c r="Y4">
-        <v>7.9097400000000002</v>
-      </c>
-      <c r="Z4">
-        <v>8.3754399999999993</v>
-      </c>
-      <c r="AA4">
-        <v>8.5328999999999997</v>
-      </c>
-      <c r="AB4">
-        <v>9.6984100000000009</v>
-      </c>
-      <c r="AC4">
-        <v>9.4666700000000006</v>
-      </c>
-      <c r="AD4">
         <v>8.6892700000000005</v>
+      </c>
+      <c r="U4" t="s">
+        <v>98</v>
+      </c>
+      <c r="V4" t="s">
+        <v>99</v>
+      </c>
+      <c r="W4" t="s">
+        <v>100</v>
+      </c>
+      <c r="X4" t="s">
+        <v>101</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>102</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>103</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>104</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>105</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>106</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:30">
@@ -741,7 +1042,7 @@
       </c>
       <c r="D5">
         <f>INDEX(J2:S11,10-H5,H4+1)</f>
-        <v>1.1240209299999999</v>
+        <v>1.8192600000000001</v>
       </c>
       <c r="G5" t="s">
         <v>12</v>
@@ -751,64 +1052,64 @@
         <v>1</v>
       </c>
       <c r="J5" s="1">
-        <v>60</v>
+        <v>5.15306</v>
       </c>
       <c r="K5" s="1">
-        <v>61</v>
+        <v>6.0157499999999997</v>
       </c>
       <c r="L5" s="1">
-        <v>62</v>
+        <v>7.4549200000000004</v>
       </c>
       <c r="M5" s="1">
-        <v>63</v>
+        <v>7.2142900000000001</v>
       </c>
       <c r="N5" s="1">
-        <v>64</v>
+        <v>7.8365499999999999</v>
       </c>
       <c r="O5" s="1">
-        <v>65</v>
+        <v>7.8296000000000001</v>
       </c>
       <c r="P5" s="1">
-        <v>66</v>
+        <v>7.1428599999999998</v>
       </c>
       <c r="Q5" s="1">
-        <v>67</v>
+        <v>7.3333300000000001</v>
       </c>
       <c r="R5" s="1">
-        <v>68</v>
+        <v>7.6296299999999997</v>
       </c>
       <c r="S5" s="1">
-        <v>69</v>
-      </c>
-      <c r="U5">
-        <v>5.15306</v>
-      </c>
-      <c r="V5">
-        <v>6.0157499999999997</v>
-      </c>
-      <c r="W5">
-        <v>7.4549200000000004</v>
-      </c>
-      <c r="X5">
-        <v>7.2142900000000001</v>
-      </c>
-      <c r="Y5">
-        <v>7.8365499999999999</v>
-      </c>
-      <c r="Z5">
-        <v>7.8296000000000001</v>
-      </c>
-      <c r="AA5">
-        <v>7.1428599999999998</v>
-      </c>
-      <c r="AB5">
-        <v>7.3333300000000001</v>
-      </c>
-      <c r="AC5">
-        <v>7.6296299999999997</v>
-      </c>
-      <c r="AD5">
         <v>7.7142900000000001</v>
+      </c>
+      <c r="U5" t="s">
+        <v>88</v>
+      </c>
+      <c r="V5" t="s">
+        <v>89</v>
+      </c>
+      <c r="W5" t="s">
+        <v>90</v>
+      </c>
+      <c r="X5" t="s">
+        <v>91</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>92</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>93</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>94</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>95</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>96</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:30">
@@ -822,126 +1123,126 @@
         <v>6.29</v>
       </c>
       <c r="J6" s="1">
-        <v>50</v>
+        <v>4.1310799999999999</v>
       </c>
       <c r="K6" s="1">
-        <v>51</v>
+        <v>4.7524300000000004</v>
       </c>
       <c r="L6" s="1">
-        <v>52</v>
+        <v>5.3337199999999996</v>
       </c>
       <c r="M6" s="1">
-        <v>53</v>
+        <v>5.3390399999999998</v>
       </c>
       <c r="N6" s="1">
-        <v>54</v>
+        <v>6.5378800000000004</v>
       </c>
       <c r="O6" s="1">
-        <v>55</v>
+        <v>7.2430599999999998</v>
       </c>
       <c r="P6" s="1">
-        <v>56</v>
+        <v>6.96</v>
       </c>
       <c r="Q6" s="1">
-        <v>57</v>
+        <v>6.7254899999999997</v>
       </c>
       <c r="R6" s="1">
-        <v>58</v>
+        <v>6.4444499999999998</v>
       </c>
       <c r="S6" s="1">
-        <v>59</v>
-      </c>
-      <c r="U6">
-        <v>4.1310799999999999</v>
-      </c>
-      <c r="V6">
-        <v>4.7524300000000004</v>
-      </c>
-      <c r="W6">
-        <v>5.3337199999999996</v>
-      </c>
-      <c r="X6">
-        <v>5.3390399999999998</v>
-      </c>
-      <c r="Y6">
-        <v>6.5378800000000004</v>
-      </c>
-      <c r="Z6">
-        <v>7.2430599999999998</v>
-      </c>
-      <c r="AA6">
-        <v>6.96</v>
-      </c>
-      <c r="AB6">
-        <v>6.7254899999999997</v>
-      </c>
-      <c r="AC6">
-        <v>6.4444499999999998</v>
-      </c>
-      <c r="AD6">
         <v>6.93398</v>
+      </c>
+      <c r="U6" t="s">
+        <v>78</v>
+      </c>
+      <c r="V6" t="s">
+        <v>79</v>
+      </c>
+      <c r="W6" t="s">
+        <v>80</v>
+      </c>
+      <c r="X6" t="s">
+        <v>81</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>82</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>83</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>84</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>85</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>86</v>
+      </c>
+      <c r="AD6" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:30">
       <c r="J7" s="1">
-        <v>40</v>
+        <v>3.9420600000000001</v>
       </c>
       <c r="K7" s="1">
-        <v>41</v>
+        <v>3.8097400000000001</v>
       </c>
       <c r="L7" s="1">
-        <v>42</v>
+        <v>4.2846299999999999</v>
       </c>
       <c r="M7" s="1">
-        <v>43</v>
+        <v>5.0022000000000002</v>
       </c>
       <c r="N7" s="1">
-        <v>44</v>
+        <v>5.2476200000000004</v>
       </c>
       <c r="O7" s="1">
-        <v>45</v>
+        <v>4.6969700000000003</v>
       </c>
       <c r="P7" s="1">
-        <v>46</v>
+        <v>4.6478000000000002</v>
       </c>
       <c r="Q7" s="1">
-        <v>47</v>
+        <v>5.7160500000000001</v>
       </c>
       <c r="R7" s="1">
-        <v>48</v>
+        <v>5.88889</v>
       </c>
       <c r="S7" s="1">
-        <v>49</v>
-      </c>
-      <c r="U7">
-        <v>3.9420600000000001</v>
-      </c>
-      <c r="V7">
-        <v>3.8097400000000001</v>
-      </c>
-      <c r="W7">
-        <v>4.2846299999999999</v>
-      </c>
-      <c r="X7">
-        <v>5.0022000000000002</v>
-      </c>
-      <c r="Y7">
-        <v>5.2476200000000004</v>
-      </c>
-      <c r="Z7">
-        <v>4.6969700000000003</v>
-      </c>
-      <c r="AA7">
-        <v>4.6478000000000002</v>
-      </c>
-      <c r="AB7">
-        <v>5.7160500000000001</v>
-      </c>
-      <c r="AC7">
-        <v>5.88889</v>
-      </c>
-      <c r="AD7">
         <v>5.3121</v>
+      </c>
+      <c r="U7" t="s">
+        <v>68</v>
+      </c>
+      <c r="V7" t="s">
+        <v>69</v>
+      </c>
+      <c r="W7" t="s">
+        <v>70</v>
+      </c>
+      <c r="X7" t="s">
+        <v>71</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>73</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>74</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC7" t="s">
+        <v>76</v>
+      </c>
+      <c r="AD7" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:30">
@@ -953,64 +1254,64 @@
         <v>12.5</v>
       </c>
       <c r="J8" s="1">
-        <v>30</v>
+        <v>3.23529</v>
       </c>
       <c r="K8" s="1">
-        <v>31</v>
+        <v>2.8014199999999998</v>
       </c>
       <c r="L8" s="1">
-        <v>32</v>
+        <v>2.9716300000000002</v>
       </c>
       <c r="M8" s="1">
-        <v>33</v>
+        <v>3.5714299999999999</v>
       </c>
       <c r="N8" s="1">
-        <v>34</v>
+        <v>3.5628099999999998</v>
       </c>
       <c r="O8" s="1">
-        <v>35</v>
+        <v>3.6330900000000002</v>
       </c>
       <c r="P8" s="1">
-        <v>36</v>
+        <v>3</v>
       </c>
       <c r="Q8" s="1">
-        <v>37</v>
+        <v>4.2415900000000004</v>
       </c>
       <c r="R8" s="1">
-        <v>38</v>
+        <v>3.9317299999999999</v>
       </c>
       <c r="S8" s="1">
-        <v>39</v>
-      </c>
-      <c r="U8">
-        <v>3.23529</v>
-      </c>
-      <c r="V8">
-        <v>2.8014199999999998</v>
-      </c>
-      <c r="W8">
-        <v>2.9716300000000002</v>
-      </c>
-      <c r="X8">
-        <v>3.5714299999999999</v>
-      </c>
-      <c r="Y8">
-        <v>3.5628099999999998</v>
-      </c>
-      <c r="Z8">
-        <v>3.6330900000000002</v>
-      </c>
-      <c r="AA8">
-        <v>3</v>
-      </c>
-      <c r="AB8">
-        <v>4.2415900000000004</v>
-      </c>
-      <c r="AC8">
-        <v>3.9317299999999999</v>
-      </c>
-      <c r="AD8">
         <v>3.2857099999999999</v>
+      </c>
+      <c r="U8" t="s">
+        <v>58</v>
+      </c>
+      <c r="V8" t="s">
+        <v>59</v>
+      </c>
+      <c r="W8" t="s">
+        <v>60</v>
+      </c>
+      <c r="X8" t="s">
+        <v>61</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>63</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>64</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC8" t="s">
+        <v>66</v>
+      </c>
+      <c r="AD8" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:30">
@@ -1022,64 +1323,64 @@
         <v>12.5</v>
       </c>
       <c r="J9" s="1">
-        <v>1.9149378500000001</v>
+        <v>2.1865800000000002</v>
       </c>
       <c r="K9" s="1">
-        <v>2.1694214299999999</v>
+        <v>1.3596699999999999</v>
       </c>
       <c r="L9" s="1">
-        <v>3</v>
+        <v>1.3777299999999999</v>
       </c>
       <c r="M9" s="1">
-        <v>23</v>
+        <v>1.6666700000000001</v>
       </c>
       <c r="N9" s="1">
-        <v>24</v>
+        <v>1.2795700000000001</v>
       </c>
       <c r="O9" s="1">
-        <v>25</v>
+        <v>2.3867400000000001</v>
       </c>
       <c r="P9" s="1">
-        <v>26</v>
+        <v>2.90055</v>
       </c>
       <c r="Q9" s="1">
-        <v>27</v>
+        <v>3.2544499999999998</v>
       </c>
       <c r="R9" s="1">
-        <v>28</v>
+        <v>2.7066699999999999</v>
       </c>
       <c r="S9" s="1">
-        <v>29</v>
-      </c>
-      <c r="U9">
-        <v>2.1865800000000002</v>
-      </c>
-      <c r="V9">
-        <v>1.3596699999999999</v>
-      </c>
-      <c r="W9">
-        <v>1.3777299999999999</v>
-      </c>
-      <c r="X9">
-        <v>1.6666700000000001</v>
-      </c>
-      <c r="Y9">
-        <v>1.2795700000000001</v>
-      </c>
-      <c r="Z9">
-        <v>2.3867400000000001</v>
-      </c>
-      <c r="AA9">
-        <v>2.90055</v>
-      </c>
-      <c r="AB9">
-        <v>3.2544499999999998</v>
-      </c>
-      <c r="AC9">
-        <v>2.7066699999999999</v>
-      </c>
-      <c r="AD9">
         <v>2.1352899999999999</v>
+      </c>
+      <c r="U9" t="s">
+        <v>48</v>
+      </c>
+      <c r="V9" t="s">
+        <v>49</v>
+      </c>
+      <c r="W9" t="s">
+        <v>50</v>
+      </c>
+      <c r="X9" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>52</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>53</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>55</v>
+      </c>
+      <c r="AC9" t="s">
+        <v>56</v>
+      </c>
+      <c r="AD9" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:30">
@@ -1091,64 +1392,64 @@
         <v>12.5</v>
       </c>
       <c r="J10" s="1">
-        <v>1.1240209299999999</v>
+        <v>1.8192600000000001</v>
       </c>
       <c r="K10" s="1">
-        <v>1.6814620499999999</v>
+        <v>1.0701799999999999</v>
       </c>
       <c r="L10" s="1">
-        <v>1.70000017</v>
+        <v>1.0740700000000001</v>
       </c>
       <c r="M10" s="1">
-        <v>13</v>
+        <v>1.0238700000000001</v>
       </c>
       <c r="N10" s="1">
-        <v>14</v>
+        <v>0.49019000000000001</v>
       </c>
       <c r="O10" s="1">
-        <v>15</v>
+        <v>0.62963000000000002</v>
       </c>
       <c r="P10" s="1">
-        <v>16</v>
+        <v>1.4512100000000001</v>
       </c>
       <c r="Q10" s="1">
-        <v>17</v>
+        <v>1.8676600000000001</v>
       </c>
       <c r="R10" s="1">
-        <v>18</v>
+        <v>2.44279</v>
       </c>
       <c r="S10" s="1">
-        <v>19</v>
-      </c>
-      <c r="U10">
-        <v>1.8192600000000001</v>
-      </c>
-      <c r="V10">
-        <v>1.0701799999999999</v>
-      </c>
-      <c r="W10">
-        <v>1.0740700000000001</v>
-      </c>
-      <c r="X10">
-        <v>1.0238700000000001</v>
-      </c>
-      <c r="Y10">
-        <v>0.49019000000000001</v>
-      </c>
-      <c r="Z10">
-        <v>0.62963000000000002</v>
-      </c>
-      <c r="AA10">
-        <v>1.4512100000000001</v>
-      </c>
-      <c r="AB10">
-        <v>1.8676600000000001</v>
-      </c>
-      <c r="AC10">
-        <v>2.44279</v>
-      </c>
-      <c r="AD10">
         <v>2.0850900000000001</v>
+      </c>
+      <c r="U10" t="s">
+        <v>38</v>
+      </c>
+      <c r="V10" t="s">
+        <v>39</v>
+      </c>
+      <c r="W10" t="s">
+        <v>40</v>
+      </c>
+      <c r="X10" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB10" t="s">
+        <v>45</v>
+      </c>
+      <c r="AC10" t="s">
+        <v>46</v>
+      </c>
+      <c r="AD10" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:30">
@@ -1160,64 +1461,64 @@
         <v>3.2250000000000001</v>
       </c>
       <c r="J11" s="1">
-        <v>0</v>
+        <v>1.30769</v>
       </c>
       <c r="K11" s="1">
-        <v>0.5</v>
+        <v>1.1126199999999999</v>
       </c>
       <c r="L11" s="1">
-        <v>1</v>
+        <v>1.0465100000000001</v>
       </c>
       <c r="M11" s="1">
-        <v>3</v>
+        <v>0.53846000000000005</v>
       </c>
       <c r="N11" s="1">
-        <v>4</v>
+        <v>8.3059999999999995E-2</v>
       </c>
       <c r="O11" s="1">
-        <v>5</v>
+        <v>8.8499999999999995E-2</v>
       </c>
       <c r="P11" s="1">
-        <v>6</v>
+        <v>0.79310000000000003</v>
       </c>
       <c r="Q11" s="1">
-        <v>7</v>
+        <v>1.4761899999999999</v>
       </c>
       <c r="R11" s="1">
-        <v>8</v>
+        <v>1.81481</v>
       </c>
       <c r="S11" s="1">
-        <v>9</v>
-      </c>
-      <c r="U11">
-        <v>1.30769</v>
-      </c>
-      <c r="V11">
-        <v>1.1126199999999999</v>
-      </c>
-      <c r="W11">
-        <v>1.0465100000000001</v>
-      </c>
-      <c r="X11">
-        <v>0.53846000000000005</v>
-      </c>
-      <c r="Y11">
-        <v>8.3059999999999995E-2</v>
-      </c>
-      <c r="Z11">
-        <v>8.8499999999999995E-2</v>
-      </c>
-      <c r="AA11">
-        <v>0.79310000000000003</v>
-      </c>
-      <c r="AB11">
-        <v>1.4761899999999999</v>
-      </c>
-      <c r="AC11">
-        <v>1.81481</v>
-      </c>
-      <c r="AD11">
         <v>1.9213499999999999</v>
+      </c>
+      <c r="U11" t="s">
+        <v>28</v>
+      </c>
+      <c r="V11" t="s">
+        <v>29</v>
+      </c>
+      <c r="W11" t="s">
+        <v>30</v>
+      </c>
+      <c r="X11" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>35</v>
+      </c>
+      <c r="AC11" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD11" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:30">
@@ -1320,7 +1621,7 @@
       </c>
       <c r="B25">
         <f>D2*B21+IF(G12="Top-right triangle",D3,D5)*B22+D4*B23</f>
-        <v>1.71828627936</v>
+        <v>1.3896725599999997</v>
       </c>
     </row>
   </sheetData>

</xml_diff>